<commit_message>
Add questions algorithm corrected
</commit_message>
<xml_diff>
--- a/src/Master.xlsx
+++ b/src/Master.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C_Bank" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C++_Bank" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet'!$A$1:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'C++_Bank'!$A$1:$E$8</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -482,18 +483,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" ht="18.6" customFormat="1" customHeight="1" s="3" thickBot="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Serial No.</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Question Description</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Topic</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>Answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>This is sample C question ';</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr"/>
+      <c r="E2" s="1" t="inlineStr"/>
+      <c r="F2" s="1" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="80.88671875" customWidth="1" style="8" min="2" max="2"/>
-    <col width="14.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="11.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="8.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="80.85546875" customWidth="1" style="8" min="2" max="2"/>
+    <col width="14.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8.7109375" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -657,7 +727,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="16.8" customHeight="1">
+    <row r="5" ht="16.9" customHeight="1">
       <c r="A5" t="n">
         <v>4</v>
       </c>
@@ -701,7 +771,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="403.2" customHeight="1">
+    <row r="6" ht="403.15" customHeight="1">
       <c r="A6" t="n">
         <v>5</v>
       </c>
@@ -1161,7 +1231,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="403.2" customHeight="1">
+    <row r="17" ht="403.15" customHeight="1">
       <c r="A17" s="1" t="n">
         <v>17</v>
       </c>
@@ -1597,7 +1667,7 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="25.8" customHeight="1">
+    <row r="24" ht="25.9" customHeight="1">
       <c r="A24" s="1" t="n">
         <v>24</v>
       </c>
@@ -1900,7 +1970,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="100.8" customHeight="1">
+    <row r="29" ht="100.9" customHeight="1">
       <c r="A29" s="1" t="n">
         <v>29</v>
       </c>
@@ -1997,7 +2067,7 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="100.8" customHeight="1">
+    <row r="31" ht="100.9" customHeight="1">
       <c r="A31" s="1" t="n">
         <v>31</v>
       </c>
@@ -2095,7 +2165,7 @@
         </is>
       </c>
     </row>
-    <row r="33" ht="319.2" customHeight="1">
+    <row r="33" ht="319.15" customHeight="1">
       <c r="A33" s="1" t="n">
         <v>33</v>
       </c>
@@ -2342,7 +2412,7 @@
         </is>
       </c>
     </row>
-    <row r="38" ht="268.8" customHeight="1">
+    <row r="38" ht="268.9" customHeight="1">
       <c r="A38" s="1" t="n">
         <v>38</v>
       </c>
@@ -2389,7 +2459,7 @@
         </is>
       </c>
     </row>
-    <row r="39" ht="16.8" customHeight="1">
+    <row r="39" ht="16.9" customHeight="1">
       <c r="A39" s="1" t="n">
         <v>39</v>
       </c>
@@ -2459,7 +2529,7 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="37.8" customHeight="1">
+    <row r="41" ht="37.9" customHeight="1">
       <c r="A41" s="1" t="n">
         <v>41</v>
       </c>
@@ -2561,7 +2631,7 @@
         </is>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="16.5" customHeight="1">
       <c r="A44" s="1" t="n">
         <v>44</v>
       </c>
@@ -2595,7 +2665,7 @@
         </is>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="16.5" customHeight="1">
       <c r="A45" s="1" t="n">
         <v>45</v>
       </c>
@@ -2629,7 +2699,7 @@
         </is>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="16.5" customHeight="1">
       <c r="A46" s="1" t="n">
         <v>46</v>
       </c>
@@ -2663,7 +2733,7 @@
         </is>
       </c>
     </row>
-    <row r="47">
+    <row r="47" ht="16.5" customHeight="1">
       <c r="A47" s="1" t="n">
         <v>47</v>
       </c>
@@ -2697,7 +2767,7 @@
         </is>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="16.5" customHeight="1">
       <c r="A48" s="1" t="n">
         <v>48</v>
       </c>
@@ -2731,7 +2801,7 @@
         </is>
       </c>
     </row>
-    <row r="49">
+    <row r="49" ht="16.5" customHeight="1">
       <c r="A49" s="1" t="n">
         <v>49</v>
       </c>

</xml_diff>